<commit_message>
feat: select tps at pengelolaan data
</commit_message>
<xml_diff>
--- a/database/bawaslu.xlsx
+++ b/database/bawaslu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ammar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ammar\Documents\bawaslu-surabaya-fix\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF946DE-BA2D-453B-828A-D2B624B94C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF68A08-5171-484B-8FDA-8EE65DE6E065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{88D03145-8660-4DCE-9892-C69239095B9A}"/>
+    <workbookView xWindow="4704" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{88D03145-8660-4DCE-9892-C69239095B9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BBAB435-B016-46D3-ADF4-3D83CF2E1F45}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +485,7 @@
     </row>
     <row r="2" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -494,7 +494,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
@@ -511,7 +511,7 @@
     </row>
     <row r="3" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -520,7 +520,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="2">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
@@ -537,7 +537,7 @@
     </row>
     <row r="4" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -546,7 +546,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="2">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="5" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -572,7 +572,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="2">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>10</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="6" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -598,7 +598,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>10</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="7" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -624,7 +624,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="2">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>10</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="8" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -650,7 +650,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="2">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>10</v>
@@ -662,12 +662,12 @@
         <v>2</v>
       </c>
       <c r="H8" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -676,7 +676,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="2">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>10</v>
@@ -688,12 +688,12 @@
         <v>2</v>
       </c>
       <c r="H9" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -702,7 +702,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="2">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>10</v>
@@ -714,12 +714,12 @@
         <v>2</v>
       </c>
       <c r="H10" s="2">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
@@ -728,7 +728,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="2">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>10</v>
@@ -740,12 +740,12 @@
         <v>2</v>
       </c>
       <c r="H11" s="2">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
@@ -754,7 +754,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="2">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>10</v>
@@ -766,12 +766,12 @@
         <v>2</v>
       </c>
       <c r="H12" s="2">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
@@ -780,7 +780,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="2">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>10</v>
@@ -792,12 +792,12 @@
         <v>2</v>
       </c>
       <c r="H13" s="2">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>8</v>
@@ -806,7 +806,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="2">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>10</v>
@@ -818,12 +818,12 @@
         <v>2</v>
       </c>
       <c r="H14" s="2">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
@@ -832,7 +832,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="2">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>10</v>
@@ -844,12 +844,12 @@
         <v>2</v>
       </c>
       <c r="H15" s="2">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
@@ -858,7 +858,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="2">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>10</v>
@@ -870,10 +870,13 @@
         <v>2</v>
       </c>
       <c r="H16" s="2">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H16">
+    <sortCondition ref="H5:H16"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>